<commit_message>
Addition of championship box plots
</commit_message>
<xml_diff>
--- a/plotly_aths_dashboard/World Rankings Scrape Tracker.xlsx
+++ b/plotly_aths_dashboard/World Rankings Scrape Tracker.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/newmac/PycharmProjects/results-webanalytics/plotly_aths_dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBBB504-8E38-0A40-BD7D-E3CCCB0E2785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACF86B0-8F26-0347-B5B0-547715E5C2F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16340" xr2:uid="{3A95C0CB-D1C2-2C4A-A2A0-01EBC986003A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="WC_2022" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -508,7 +508,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A28"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>